<commit_message>
document matching is done perfectly
</commit_message>
<xml_diff>
--- a/Back-End/API.xlsx
+++ b/Back-End/API.xlsx
@@ -18,9 +18,78 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <r>
+      <t xml:space="preserve">           </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF006100"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">API Name </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>API URL</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">               Body Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      Response Data</t>
+  </si>
+  <si>
+    <t>Example</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               SignUp </t>
+  </si>
+  <si>
+    <t>http://localhost:5555/api/users/signup</t>
+  </si>
+  <si>
+    <t>name, email, mobile, password</t>
+  </si>
+  <si>
+    <t>{name, email, mobile, image, password, docs, signed}</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,13 +97,49 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="4" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -46,13 +151,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -331,12 +443,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="3" width="40.7109375" customWidth="1"/>
+    <col min="4" max="4" width="50.7109375" customWidth="1"/>
+    <col min="5" max="5" width="30.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>